<commit_message>
Created a back up for the previous application and appended latest application by Falogme 3-2-16
</commit_message>
<xml_diff>
--- a/hcmselenium/src/hcm/testdata/SampleTestData.xlsx
+++ b/hcmselenium/src/hcm/testdata/SampleTestData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Manage Performance" sheetId="7" r:id="rId1"/>
     <sheet name="Compensation Management" sheetId="9" r:id="rId2"/>
+    <sheet name="Configure Offerings" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="39">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -133,6 +134,15 @@
   </si>
   <si>
     <t>Absence Management</t>
+  </si>
+  <si>
+    <t>Total Compensation Statements</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>ConfigureOfferingsTest</t>
   </si>
 </sst>
 </file>
@@ -190,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -271,12 +281,193 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -325,6 +516,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -609,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FU3"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
@@ -1523,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
@@ -2387,4 +2626,902 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:FY3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="76.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" customWidth="1"/>
+    <col min="14" max="14" width="43.28515625" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" customWidth="1"/>
+    <col min="19" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" customWidth="1"/>
+    <col min="30" max="30" width="19.42578125" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" customWidth="1"/>
+    <col min="32" max="32" width="19.85546875" customWidth="1"/>
+    <col min="33" max="33" width="8.7109375" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" customWidth="1"/>
+    <col min="36" max="36" width="18.85546875" customWidth="1"/>
+    <col min="37" max="37" width="11.5703125" customWidth="1"/>
+    <col min="38" max="38" width="17.42578125" customWidth="1"/>
+    <col min="39" max="39" width="8.7109375" customWidth="1"/>
+    <col min="40" max="40" width="12.28515625" customWidth="1"/>
+    <col min="41" max="41" width="16.85546875" customWidth="1"/>
+    <col min="42" max="42" width="19.140625" customWidth="1"/>
+    <col min="43" max="43" width="11.5703125" customWidth="1"/>
+    <col min="44" max="44" width="19.140625" customWidth="1"/>
+    <col min="45" max="45" width="8.7109375" customWidth="1"/>
+    <col min="46" max="46" width="12.28515625" customWidth="1"/>
+    <col min="47" max="47" width="14.28515625" customWidth="1"/>
+    <col min="48" max="48" width="16.85546875" customWidth="1"/>
+    <col min="49" max="49" width="18.85546875" customWidth="1"/>
+    <col min="50" max="50" width="11.5703125" customWidth="1"/>
+    <col min="51" max="51" width="18.85546875" customWidth="1"/>
+    <col min="52" max="52" width="8.7109375" customWidth="1"/>
+    <col min="53" max="53" width="12.28515625" customWidth="1"/>
+    <col min="54" max="54" width="14.28515625" customWidth="1"/>
+    <col min="55" max="55" width="16.85546875" customWidth="1"/>
+    <col min="56" max="56" width="18.85546875" customWidth="1"/>
+    <col min="57" max="57" width="11.5703125" customWidth="1"/>
+    <col min="58" max="58" width="18.85546875" customWidth="1"/>
+    <col min="59" max="59" width="8.7109375" customWidth="1"/>
+    <col min="60" max="60" width="12.28515625" customWidth="1"/>
+    <col min="61" max="61" width="14.28515625" customWidth="1"/>
+    <col min="62" max="62" width="16.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.85546875" customWidth="1"/>
+    <col min="64" max="64" width="11.5703125" customWidth="1"/>
+    <col min="65" max="66" width="18.85546875" customWidth="1"/>
+    <col min="67" max="67" width="8.7109375" customWidth="1"/>
+    <col min="68" max="68" width="12.28515625" customWidth="1"/>
+    <col min="69" max="76" width="20.7109375" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" customWidth="1"/>
+    <col min="78" max="92" width="3" customWidth="1"/>
+    <col min="93" max="99" width="16.42578125" customWidth="1"/>
+    <col min="100" max="100" width="12.42578125" customWidth="1"/>
+    <col min="101" max="101" width="18.42578125" customWidth="1"/>
+    <col min="102" max="102" width="16.140625" customWidth="1"/>
+    <col min="103" max="103" width="15.5703125" customWidth="1"/>
+    <col min="104" max="105" width="14.28515625" customWidth="1"/>
+    <col min="110" max="110" width="18.42578125" customWidth="1"/>
+    <col min="111" max="111" width="14.85546875" customWidth="1"/>
+    <col min="113" max="113" width="11.42578125" customWidth="1"/>
+    <col min="114" max="114" width="12.5703125" customWidth="1"/>
+    <col min="117" max="117" width="11" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="12.7109375" customWidth="1"/>
+    <col min="121" max="121" width="16.85546875" customWidth="1"/>
+    <col min="126" max="126" width="11.42578125" customWidth="1"/>
+    <col min="128" max="128" width="13.42578125" customWidth="1"/>
+    <col min="129" max="129" width="12.5703125" customWidth="1"/>
+    <col min="130" max="130" width="12" customWidth="1"/>
+    <col min="131" max="131" width="10" customWidth="1"/>
+    <col min="137" max="137" width="10.85546875" customWidth="1"/>
+    <col min="138" max="138" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:181" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="31">
+        <v>8</v>
+      </c>
+      <c r="J1" s="22">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="22">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="22">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="1">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="1">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="1">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="1">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="1">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="1">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="1">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="1">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="1">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="1">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="1">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="1">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="1">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="1">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="1">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="1">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="1">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="1">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="1">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="1">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="1">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="1">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="1">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="1"/>
+      <c r="CP1" s="1"/>
+      <c r="CQ1" s="1"/>
+      <c r="CR1" s="1"/>
+      <c r="CS1" s="1"/>
+      <c r="CT1" s="1"/>
+      <c r="CU1" s="1"/>
+      <c r="CV1" s="1"/>
+      <c r="CW1" s="1"/>
+      <c r="CX1" s="1"/>
+      <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
+      <c r="DB1" s="1"/>
+      <c r="DC1" s="1"/>
+      <c r="DD1" s="1"/>
+      <c r="DE1" s="1"/>
+      <c r="DF1" s="1"/>
+      <c r="DG1" s="1"/>
+      <c r="DH1" s="1"/>
+      <c r="DI1" s="1"/>
+      <c r="DJ1" s="1"/>
+      <c r="DK1" s="1"/>
+      <c r="DL1" s="1"/>
+      <c r="DM1" s="1"/>
+      <c r="DN1" s="1"/>
+      <c r="DO1" s="1"/>
+      <c r="DP1" s="1"/>
+      <c r="DQ1" s="1"/>
+      <c r="DR1" s="1"/>
+      <c r="DS1" s="1"/>
+      <c r="DT1" s="1"/>
+      <c r="DU1" s="1"/>
+      <c r="DV1" s="1"/>
+      <c r="DW1" s="1"/>
+      <c r="DX1" s="1"/>
+      <c r="DY1" s="1"/>
+      <c r="DZ1" s="1"/>
+      <c r="EA1" s="1"/>
+      <c r="EB1" s="1"/>
+      <c r="EC1" s="1"/>
+      <c r="ED1" s="1"/>
+      <c r="EE1" s="1"/>
+      <c r="EF1" s="1"/>
+      <c r="EG1" s="1"/>
+      <c r="EH1" s="1"/>
+      <c r="EI1" s="1"/>
+      <c r="EJ1" s="1"/>
+      <c r="EK1" s="1"/>
+      <c r="EL1" s="1"/>
+      <c r="EM1" s="1"/>
+      <c r="EN1" s="1"/>
+      <c r="EO1" s="1"/>
+      <c r="EP1" s="1"/>
+      <c r="EQ1" s="1"/>
+      <c r="ER1" s="1"/>
+      <c r="ES1" s="1"/>
+      <c r="ET1" s="1"/>
+      <c r="EU1" s="1"/>
+      <c r="EV1" s="1"/>
+      <c r="EW1" s="1"/>
+      <c r="EX1" s="1"/>
+      <c r="EY1" s="1"/>
+      <c r="EZ1" s="1"/>
+      <c r="FA1" s="1"/>
+      <c r="FB1" s="1"/>
+      <c r="FC1" s="1"/>
+      <c r="FD1" s="1"/>
+      <c r="FE1" s="1"/>
+      <c r="FF1" s="1"/>
+      <c r="FG1" s="1"/>
+      <c r="FH1" s="1"/>
+      <c r="FI1" s="1"/>
+      <c r="FJ1" s="1"/>
+      <c r="FK1" s="1"/>
+      <c r="FL1" s="1"/>
+      <c r="FM1" s="1"/>
+      <c r="FN1" s="1"/>
+      <c r="FO1" s="1"/>
+      <c r="FP1" s="1"/>
+    </row>
+    <row r="2" spans="1:181" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
+      <c r="BN2" s="8"/>
+      <c r="BO2" s="8"/>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="8"/>
+      <c r="CB2" s="8"/>
+      <c r="CC2" s="8"/>
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="8"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="8"/>
+      <c r="CH2" s="8"/>
+      <c r="CI2" s="8"/>
+      <c r="CJ2" s="8"/>
+      <c r="CK2" s="8"/>
+      <c r="CL2" s="8"/>
+      <c r="CM2" s="8"/>
+      <c r="CN2" s="8"/>
+      <c r="CO2" s="8"/>
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="8"/>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8"/>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
+      <c r="CZ2" s="8"/>
+      <c r="DA2" s="8"/>
+      <c r="DB2" s="8"/>
+      <c r="DC2" s="8"/>
+      <c r="DD2" s="8"/>
+      <c r="DE2" s="8"/>
+      <c r="DF2" s="8"/>
+      <c r="DG2" s="8"/>
+      <c r="DH2" s="8"/>
+      <c r="DI2" s="8"/>
+      <c r="DJ2" s="8"/>
+      <c r="DK2" s="8"/>
+      <c r="DL2" s="8"/>
+      <c r="DM2" s="8"/>
+      <c r="DN2" s="8"/>
+      <c r="DO2" s="8"/>
+      <c r="DP2" s="8"/>
+      <c r="DQ2" s="8"/>
+      <c r="DR2" s="8"/>
+      <c r="DS2" s="8"/>
+      <c r="DT2" s="8"/>
+      <c r="DU2" s="8"/>
+      <c r="DV2" s="8"/>
+      <c r="DW2" s="8"/>
+      <c r="DX2" s="8"/>
+      <c r="DY2" s="8"/>
+      <c r="DZ2" s="8"/>
+      <c r="EA2" s="8"/>
+      <c r="EB2" s="8"/>
+      <c r="EC2" s="8"/>
+      <c r="ED2" s="8"/>
+      <c r="EE2" s="8"/>
+      <c r="EF2" s="8"/>
+      <c r="EG2" s="8"/>
+      <c r="EH2" s="8"/>
+      <c r="EI2" s="8"/>
+      <c r="EJ2" s="8"/>
+      <c r="EK2" s="8"/>
+      <c r="EL2" s="8"/>
+      <c r="EM2" s="8"/>
+      <c r="EN2" s="8"/>
+      <c r="EO2" s="8"/>
+      <c r="EP2" s="8"/>
+      <c r="EQ2" s="8"/>
+      <c r="ER2" s="8"/>
+      <c r="ES2" s="8"/>
+      <c r="ET2" s="8"/>
+      <c r="EU2" s="8"/>
+      <c r="EV2" s="8"/>
+      <c r="EW2" s="8"/>
+      <c r="EX2" s="8"/>
+      <c r="EY2" s="8"/>
+      <c r="EZ2" s="8"/>
+      <c r="FA2" s="8"/>
+      <c r="FB2" s="8"/>
+      <c r="FC2" s="8"/>
+      <c r="FD2" s="8"/>
+      <c r="FE2" s="8"/>
+      <c r="FF2" s="8"/>
+      <c r="FG2" s="8"/>
+      <c r="FH2" s="8"/>
+      <c r="FI2" s="8"/>
+      <c r="FJ2" s="8"/>
+      <c r="FK2" s="8"/>
+      <c r="FL2" s="8"/>
+      <c r="FM2" s="8"/>
+      <c r="FN2" s="8"/>
+      <c r="FO2" s="8"/>
+      <c r="FP2" s="8"/>
+      <c r="FQ2" s="8"/>
+      <c r="FR2" s="8"/>
+      <c r="FS2" s="8"/>
+      <c r="FT2" s="8"/>
+      <c r="FU2" s="8"/>
+      <c r="FV2" s="8"/>
+      <c r="FW2" s="8"/>
+      <c r="FX2" s="8"/>
+      <c r="FY2" s="8"/>
+    </row>
+    <row r="3" spans="1:181" s="7" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="3"/>
+      <c r="AY3" s="5"/>
+      <c r="AZ3" s="3"/>
+      <c r="BA3" s="3"/>
+      <c r="BB3" s="3"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="5"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3" s="3"/>
+      <c r="BJ3" s="3"/>
+      <c r="BK3" s="3"/>
+      <c r="BL3" s="3"/>
+      <c r="BM3" s="5"/>
+      <c r="BN3" s="3"/>
+      <c r="BO3" s="3"/>
+      <c r="BP3" s="3"/>
+      <c r="BQ3" s="3"/>
+      <c r="BR3" s="11"/>
+      <c r="BS3" s="3"/>
+      <c r="BT3" s="3"/>
+      <c r="BU3" s="3"/>
+      <c r="BV3" s="6"/>
+      <c r="BW3" s="6"/>
+      <c r="BX3" s="6"/>
+      <c r="BY3" s="6"/>
+      <c r="BZ3" s="6"/>
+      <c r="CA3" s="6"/>
+      <c r="CB3" s="6"/>
+      <c r="CC3" s="6"/>
+      <c r="CD3" s="6"/>
+      <c r="CE3" s="6"/>
+      <c r="CF3" s="6"/>
+      <c r="CG3" s="6"/>
+      <c r="CH3" s="6"/>
+      <c r="CI3" s="6"/>
+      <c r="CJ3" s="6"/>
+      <c r="CK3" s="6"/>
+      <c r="CL3" s="6"/>
+      <c r="CM3" s="6"/>
+      <c r="CN3" s="6"/>
+      <c r="CO3" s="6"/>
+      <c r="CP3" s="3"/>
+      <c r="CQ3" s="3"/>
+      <c r="CR3" s="6"/>
+      <c r="CS3" s="3"/>
+      <c r="CT3" s="3"/>
+      <c r="CU3" s="3"/>
+      <c r="CV3" s="3"/>
+      <c r="CW3" s="6"/>
+      <c r="CX3" s="6"/>
+      <c r="CY3" s="6"/>
+      <c r="CZ3" s="6"/>
+      <c r="DA3" s="6"/>
+      <c r="DB3" s="6"/>
+      <c r="DC3" s="6"/>
+      <c r="DD3" s="6"/>
+      <c r="DE3" s="6"/>
+      <c r="DF3" s="6"/>
+      <c r="DG3" s="6"/>
+      <c r="DH3" s="6"/>
+      <c r="DI3" s="6"/>
+      <c r="DJ3" s="4"/>
+      <c r="DK3" s="3"/>
+      <c r="DL3" s="3"/>
+      <c r="DM3" s="3"/>
+      <c r="DN3" s="3"/>
+      <c r="DO3" s="3"/>
+      <c r="DP3" s="3"/>
+      <c r="DQ3" s="3"/>
+      <c r="DR3" s="3"/>
+      <c r="DS3" s="3"/>
+      <c r="DT3" s="3"/>
+      <c r="DU3" s="3"/>
+      <c r="DV3" s="3"/>
+      <c r="DW3" s="3"/>
+      <c r="DX3" s="3"/>
+      <c r="DY3" s="3"/>
+      <c r="DZ3" s="3"/>
+      <c r="EA3" s="3"/>
+      <c r="EB3" s="3"/>
+      <c r="EC3" s="3"/>
+      <c r="ED3" s="3"/>
+      <c r="EE3" s="3"/>
+      <c r="EF3" s="3"/>
+      <c r="EG3" s="3"/>
+      <c r="EH3" s="3"/>
+      <c r="EI3" s="3"/>
+      <c r="EJ3" s="3"/>
+      <c r="EK3" s="6"/>
+      <c r="EL3" s="6"/>
+      <c r="EM3" s="6"/>
+      <c r="EN3" s="6"/>
+      <c r="EO3" s="6"/>
+      <c r="EP3" s="6"/>
+      <c r="EQ3" s="6"/>
+      <c r="ER3" s="6"/>
+      <c r="ES3" s="6"/>
+      <c r="ET3" s="6"/>
+      <c r="EU3" s="4"/>
+      <c r="EV3" s="3"/>
+      <c r="EW3" s="3"/>
+      <c r="EX3" s="3"/>
+      <c r="EY3" s="3"/>
+      <c r="EZ3" s="3"/>
+      <c r="FA3" s="3"/>
+      <c r="FB3" s="3"/>
+      <c r="FC3" s="3"/>
+      <c r="FD3" s="3"/>
+      <c r="FE3" s="3"/>
+      <c r="FF3" s="3"/>
+      <c r="FG3" s="3"/>
+      <c r="FH3" s="3"/>
+      <c r="FI3" s="3"/>
+      <c r="FJ3" s="3"/>
+      <c r="FK3" s="3"/>
+      <c r="FL3" s="3"/>
+      <c r="FM3" s="3"/>
+      <c r="FN3" s="3"/>
+      <c r="FO3" s="3"/>
+      <c r="FP3" s="3"/>
+      <c r="FQ3" s="3"/>
+      <c r="FR3" s="3"/>
+      <c r="FS3" s="3"/>
+      <c r="FT3" s="3"/>
+      <c r="FU3" s="3"/>
+      <c r="FV3" s="3"/>
+      <c r="FW3" s="3"/>
+      <c r="FX3" s="3"/>
+      <c r="FY3" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>